<commit_message>
Added LHP, LP, SKHD, Edit Personel
</commit_message>
<xml_diff>
--- a/FORMAT CATPERS.xlsx
+++ b/FORMAT CATPERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProjekGawian\SICAPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F88ECE8-A83E-42E1-986B-EA5749681383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71F417B-FB85-40BA-8C40-1B688DC6C94B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="690" yWindow="1860" windowWidth="11520" windowHeight="7995" activeTab="1" xr2:uid="{A1CDF61C-E919-4592-BC50-D9E8CABB0334}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{A1CDF61C-E919-4592-BC50-D9E8CABB0334}"/>
   </bookViews>
   <sheets>
     <sheet name="CATPERS " sheetId="1" r:id="rId1"/>
@@ -692,6 +692,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,7 +729,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1232,101 +1232,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777AD3CE-E812-40A2-B339-D12343EECE7D}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31" t="s">
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1336,9 +1336,9 @@
       <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="34"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="35"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
@@ -1459,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14E580F-8BDB-4929-A7AF-A9D12D5EC6AC}">
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1487,11 +1487,11 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
     </row>
@@ -1504,34 +1504,34 @@
       <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="39" t="s">
+      <c r="H5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D6" s="9"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="42" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1543,27 +1543,27 @@
       <c r="E9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="42" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="41" t="s">
+      <c r="I9" s="42" t="s">
         <v>39</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="42"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
@@ -1573,16 +1573,16 @@
       <c r="E10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="42"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="42"/>
+      <c r="K10" s="43"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="17">

</xml_diff>